<commit_message>
message in cart code while trasfering
</commit_message>
<xml_diff>
--- a/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
+++ b/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2 archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFF566A-A2F7-481D-8811-256D2F6CA8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4344A4CE-AB43-4590-9A1A-5E557EC108F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
+    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="153">
   <si>
     <t>Value</t>
   </si>
@@ -491,22 +491,6 @@
     <t>CONN RCPT VERT 1x5 POS 0.1"</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Teensy 4.1 Devel Board </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>With Ethernet</t>
-    </r>
-  </si>
-  <si>
     <t>U1-Rcpt 1/2</t>
   </si>
   <si>
@@ -514,6 +498,15 @@
   </si>
   <si>
     <t>U1-Rcpt 4</t>
+  </si>
+  <si>
+    <t>Sq hole/short lead/flat side/-/Cathode</t>
+  </si>
+  <si>
+    <t>Be sure to cut the 5v power jumper on the back!</t>
+  </si>
+  <si>
+    <t>Teensy 4.1 Devel Board w/ Ethernet</t>
   </si>
 </sst>
 </file>
@@ -607,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -657,6 +650,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -976,14 +978,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.109375" style="9" customWidth="1"/>
     <col min="4" max="4" width="15.21875" style="9" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" style="9" bestFit="1" customWidth="1"/>
@@ -1026,7 +1028,7 @@
       <c r="B2" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="20" t="s">
         <v>124</v>
       </c>
       <c r="D2" s="8"/>
@@ -1068,7 +1070,7 @@
       <c r="B4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -1101,7 +1103,9 @@
       <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="8"/>
+      <c r="H5" s="8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5">
@@ -1158,7 +1162,7 @@
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="20" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -1219,7 +1223,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="28.8">
       <c r="A11" s="5">
         <v>1</v>
       </c>
@@ -1252,8 +1256,8 @@
       <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>147</v>
+      <c r="C12" s="21" t="s">
+        <v>152</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>13</v>
@@ -1265,9 +1269,11 @@
         <v>44</v>
       </c>
       <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="H12" s="19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -1284,7 +1290,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="28.8">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -1302,7 +1308,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="28.8">
       <c r="A15" s="8">
         <v>1</v>
       </c>
@@ -1327,7 +1333,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>145</v>
@@ -1345,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>146</v>
@@ -1363,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>132</v>
@@ -1471,6 +1477,7 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Teensy pin pics, BOM pin config options
</commit_message>
<xml_diff>
--- a/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
+++ b/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2 archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B839426E-2642-4058-BFB3-FA9CE628FE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B18B10-F2E0-424B-B2B5-164D6642BCC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
+    <workbookView xWindow="4092" yWindow="2868" windowWidth="17280" windowHeight="8964" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'0.2 Export'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">BOM!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="168">
   <si>
     <t>Value</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>PJRC</t>
   </si>
   <si>
     <t>Manuf</t>
@@ -503,17 +500,66 @@
     <t>Sq hole/short lead/flat side/-/Cathode</t>
   </si>
   <si>
-    <t>Be sure to cut the 5v power jumper on the back!</t>
-  </si>
-  <si>
     <t>Teensy 4.1 Devel Board w/ Ethernet</t>
+  </si>
+  <si>
+    <t>Be sure to cut the 5v power jumper on the back (see assy instructions)</t>
+  </si>
+  <si>
+    <t>https://www.pjrc.com/store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+Ethernet Kit for Teensy 4.1</t>
+  </si>
+  <si>
+    <t>USB Host Cable For Teensy 4.1</t>
+  </si>
+  <si>
+    <t>CABLE_USB_HOST_T36</t>
+  </si>
+  <si>
+    <t>ETHERNET_KIT</t>
+  </si>
+  <si>
+    <t>U1-EthDongl</t>
+  </si>
+  <si>
+    <t>U1-USBDongl</t>
+  </si>
+  <si>
+    <t>IO Only</t>
+  </si>
+  <si>
+    <t>Sock All</t>
+  </si>
+  <si>
+    <t>Dir Con</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>C3, C4, C5, C6, C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>Only needed if not using on-board connectors</t>
+  </si>
+  <si>
+    <t>Only needed if socketting Teensy USB</t>
+  </si>
+  <si>
+    <t>Only needed if socketting Teensy Eth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,8 +586,16 @@
       <color theme="1"/>
       <name val="Courier New,courier"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,6 +632,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -603,10 +663,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -661,8 +722,27 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -976,508 +1056,750 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.77734375" style="9" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="3" width="5.21875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="3.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.109375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="24.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.44140625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="21" style="9" customWidth="1"/>
+    <col min="11" max="11" width="35.77734375" style="9" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1" ht="26.4">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:12" s="15" customFormat="1" ht="28.8">
+      <c r="A1" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="8"/>
+    <row r="2" spans="1:12">
+      <c r="A2" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
       <c r="E2" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="5">
+        <v>118</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="F4" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="8" t="s">
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="8"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" ht="43.2">
+      <c r="A11" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="5">
         <v>4</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8" t="s">
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="28.8">
+      <c r="A12" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="28.8">
+      <c r="A13" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="28.8">
+      <c r="A14" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" s="8">
+        <v>2</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="28.8">
+      <c r="A15" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="28.8">
+      <c r="A16" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="24"/>
+      <c r="B17" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="11">
+        <v>2</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="24"/>
+      <c r="B18" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="11">
+        <v>1</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="24"/>
+      <c r="B19" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="11">
+        <v>1</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="28.8">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="28.8">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G21" s="11"/>
+      <c r="H21" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="J21" s="11"/>
+      <c r="K21" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="17" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="5">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="5">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="5">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="5">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="5">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" ht="43.2">
-      <c r="A10" s="5">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="28.8">
-      <c r="A11" s="5">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8">
-      <c r="A12" s="5">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="19" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28.8">
-      <c r="A13" s="8">
-        <v>2</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.8">
-      <c r="A14" s="8">
-        <v>1</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="28.8">
-      <c r="A15" s="8">
-        <v>1</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="11">
-        <v>2</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="11">
-        <v>1</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="11">
-        <v>1</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="6">
-        <v>1</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="12" t="s">
+    <row r="23" spans="1:11">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="6">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" s="17" t="s">
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="17" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="6">
-        <v>1</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="17" t="s">
+    <row r="25" spans="1:11">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="17" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="6">
-        <v>1</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="6">
-        <v>1</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="17" t="s">
-        <v>143</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H19">
-      <sortCondition ref="B1"/>
+  <autoFilter ref="A1:K1" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K19">
+      <sortCondition ref="E1"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="H13" r:id="rId1" xr:uid="{134792E2-B64E-4FBB-BFC7-EC447106886D}"/>
+    <hyperlink ref="H20" r:id="rId2" xr:uid="{23725F89-30D6-47FA-ACEA-6838D1632F0F}"/>
+    <hyperlink ref="H21" r:id="rId3" xr:uid="{08EB66B2-5D49-472B-B4A7-8BD244E39350}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1520,40 +1842,40 @@
         <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1561,19 +1883,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -1590,10 +1912,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -1602,28 +1924,28 @@
         <v>805</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1631,19 +1953,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1660,7 +1982,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -1672,24 +1994,24 @@
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1697,16 +2019,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1728,13 +2050,13 @@
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1751,29 +2073,29 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1784,19 +2106,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1813,16 +2135,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1840,19 +2162,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1872,10 +2194,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>3</v>
@@ -1929,10 +2251,10 @@
         <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>8</v>
@@ -1958,7 +2280,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
PCB assy instructions, BOM line item #s
</commit_message>
<xml_diff>
--- a/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
+++ b/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2 archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B18B10-F2E0-424B-B2B5-164D6642BCC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776A13BC-FDD5-431B-87DF-C3252045A766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4092" yWindow="2868" windowWidth="17280" windowHeight="8964" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'0.2 Export'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">BOM!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="169">
   <si>
     <t>Value</t>
   </si>
@@ -203,9 +203,6 @@
   </si>
   <si>
     <t>CAP CER 0.1UF 50V X7R</t>
-  </si>
-  <si>
-    <t>For Teensy Ethernet connection to TeensyROM</t>
   </si>
   <si>
     <t>SWITCH-MOMENTARY-2PTH</t>
@@ -440,9 +437,6 @@
 Recommend wide package, but any of these 3 will work</t>
   </si>
   <si>
-    <t>For Teensy USB Host connection to TeensyROM</t>
-  </si>
-  <si>
     <t>CONN RCPT 6POS 0.079 PCB</t>
   </si>
   <si>
@@ -553,6 +547,41 @@
   </si>
   <si>
     <t>Only needed if socketting Teensy Eth</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For Teensy USB Host connection to TeensyROM. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Top or Bottom mount (see assy instructions)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For Teensy Ethernet connection to TeensyROM. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Top or Bottom mount (see assy instructions)</t>
+    </r>
+  </si>
+  <si>
+    <t>BOM item #</t>
   </si>
 </sst>
 </file>
@@ -667,7 +696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -739,6 +768,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1058,745 +1093,817 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="5.21875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="3.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.109375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="24.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.44140625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="21" style="9" customWidth="1"/>
-    <col min="11" max="11" width="35.77734375" style="9" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="7.6640625" style="9" customWidth="1"/>
+    <col min="2" max="4" width="5.21875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="3.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.109375" style="9" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="24.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.44140625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="21" style="9" customWidth="1"/>
+    <col min="12" max="12" width="35.77734375" style="9" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="15" customFormat="1" ht="28.8">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="5">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" ht="43.2">
+      <c r="A5" s="27">
+        <v>4</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="28.8">
+      <c r="A6" s="27">
+        <v>5</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="27">
+        <v>6</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="27">
+        <v>7</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="L8" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="27">
+        <v>8</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="G4" s="8" t="s">
+      <c r="G9" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D5" s="5">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="8"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="5">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="23" t="s">
+      <c r="L9" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="28.8">
+      <c r="A10" s="27">
+        <v>9</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="28.8">
+      <c r="A11" s="27">
+        <v>10</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="43.2">
+      <c r="A12" s="27">
+        <v>11</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="43.2">
+      <c r="A13" s="27">
+        <v>12</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="27">
+        <v>13</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="G14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="27">
+        <v>14</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="27">
+        <v>15</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="27">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" ht="43.2">
-      <c r="A11" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D11" s="5">
-        <v>4</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="28.8">
-      <c r="A12" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="28.8">
-      <c r="A13" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="19" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="28.8">
-      <c r="A14" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D14" s="8">
-        <v>2</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="28.8">
-      <c r="A15" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="8">
-        <v>1</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="28.8">
-      <c r="A16" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="8">
-        <v>1</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="24"/>
-      <c r="B17" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="11">
-        <v>2</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="18" t="s">
+        <v>142</v>
+      </c>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="24"/>
-      <c r="B18" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="11">
-        <v>1</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="F18" s="18" t="s">
+      <c r="K17" s="11"/>
+      <c r="L17" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="27">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="11">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="G18" s="11"/>
+      <c r="G18" s="18" t="s">
+        <v>143</v>
+      </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="24"/>
-      <c r="B19" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="11">
-        <v>1</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>148</v>
+      <c r="K18" s="11"/>
+      <c r="L18" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="27">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="11">
+        <v>1</v>
       </c>
       <c r="F19" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="J19" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11" t="s">
+      <c r="K19" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="28.8">
-      <c r="A20" s="24"/>
+      <c r="L19" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="28.8">
+      <c r="A20" s="27">
+        <v>19</v>
+      </c>
       <c r="B20" s="24"/>
-      <c r="C20" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11" t="s">
-        <v>157</v>
-      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" s="11"/>
       <c r="F20" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="28.8">
+      <c r="A21" s="27">
+        <v>20</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="J21" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="J20" s="11"/>
-      <c r="K20" s="16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="28.8">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="J21" s="11"/>
-      <c r="K21" s="16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="25"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="27">
+        <v>21</v>
+      </c>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
-      <c r="D22" s="6">
-        <v>1</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>85</v>
+      <c r="D22" s="25"/>
+      <c r="E22" s="6">
+        <v>1</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7" t="s">
+      <c r="H22" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K22" s="17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="24"/>
+      <c r="L22" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="27">
+        <v>22</v>
+      </c>
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>
-      <c r="D23" s="6">
-        <v>1</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="G23" s="7" t="s">
+      <c r="D23" s="24"/>
+      <c r="E23" s="6">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
-      <c r="K23" s="17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="24"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="27">
+        <v>23</v>
+      </c>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
-      <c r="D24" s="6">
-        <v>1</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>68</v>
+      <c r="D24" s="24"/>
+      <c r="E24" s="6">
+        <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="H24" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
-      <c r="K24" s="17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="24"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="27">
+        <v>24</v>
+      </c>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
-      <c r="D25" s="6">
-        <v>1</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>111</v>
+      <c r="D25" s="24"/>
+      <c r="E25" s="6">
+        <v>1</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G25" s="7"/>
+        <v>110</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
-      <c r="K25" s="17" t="s">
-        <v>142</v>
+      <c r="K25" s="7"/>
+      <c r="L25" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K19">
-      <sortCondition ref="E1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:L1" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}"/>
   <hyperlinks>
-    <hyperlink ref="H13" r:id="rId1" xr:uid="{134792E2-B64E-4FBB-BFC7-EC447106886D}"/>
-    <hyperlink ref="H20" r:id="rId2" xr:uid="{23725F89-30D6-47FA-ACEA-6838D1632F0F}"/>
-    <hyperlink ref="H21" r:id="rId3" xr:uid="{08EB66B2-5D49-472B-B4A7-8BD244E39350}"/>
+    <hyperlink ref="I10" r:id="rId1" xr:uid="{134792E2-B64E-4FBB-BFC7-EC447106886D}"/>
+    <hyperlink ref="I20" r:id="rId2" xr:uid="{23725F89-30D6-47FA-ACEA-6838D1632F0F}"/>
+    <hyperlink ref="I21" r:id="rId3" xr:uid="{08EB66B2-5D49-472B-B4A7-8BD244E39350}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -1842,40 +1949,40 @@
         <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1883,19 +1990,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -1912,10 +2019,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -1924,28 +2031,28 @@
         <v>805</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1953,19 +2060,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1982,7 +2089,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -1994,24 +2101,24 @@
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -2019,16 +2126,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2050,13 +2157,13 @@
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -2076,17 +2183,17 @@
         <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -2095,7 +2202,7 @@
         <v>44</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -2106,19 +2213,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -2135,16 +2242,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2162,19 +2269,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -2194,10 +2301,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>3</v>
@@ -2251,10 +2358,10 @@
         <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>8</v>
@@ -2280,7 +2387,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Heatsink on BOM and PCB readme
</commit_message>
<xml_diff>
--- a/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
+++ b/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2 archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776A13BC-FDD5-431B-87DF-C3252045A766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107BEB2F-C1C1-41AD-A42D-4D2F93DE04FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="174">
   <si>
     <t>Value</t>
   </si>
@@ -582,6 +582,21 @@
   </si>
   <si>
     <t>BOM item #</t>
+  </si>
+  <si>
+    <t>9a</t>
+  </si>
+  <si>
+    <t>U1 Heatsink</t>
+  </si>
+  <si>
+    <t>14x14mm Aluminum heatsink w/ Thermal Conductive Adhesive Tape</t>
+  </si>
+  <si>
+    <t>Multiple, such as:     https://www.amazon.com/Heatsink-14x14x10mm-0-55x0-55x0-39-Conductive-Dissipation/dp/B07ZC68LNM/</t>
+  </si>
+  <si>
+    <t>Optional, but recommended</t>
   </si>
 </sst>
 </file>
@@ -668,7 +683,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -691,12 +706,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -774,6 +815,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1091,10 +1138,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1463,68 +1510,70 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="28.8">
-      <c r="A11" s="27">
+      <c r="A11" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="J11" s="29"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="28.8">
+      <c r="A12" s="27">
         <v>10</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="E11" s="8">
+      <c r="B12" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="8">
         <v>2</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="43.2">
-      <c r="A12" s="27">
-        <v>11</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12" s="8">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>135</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="24" t="s">
-        <v>166</v>
+      <c r="L12" s="8" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="43.2">
       <c r="A13" s="27">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>160</v>
@@ -1539,52 +1588,54 @@
         <v>1</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>50</v>
+        <v>119</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="8"/>
+      <c r="L13" s="24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="43.2">
+      <c r="A14" s="27">
+        <v>12</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L13" s="24" t="s">
+      <c r="L14" s="24" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="27">
-        <v>13</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="5">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="27">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>160</v>
@@ -1592,33 +1643,27 @@
       <c r="C15" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="D15" s="24"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="5">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>46</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="27">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>160</v>
@@ -1631,82 +1676,90 @@
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>30</v>
+        <v>60</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>112</v>
+        <v>52</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="27">
+        <v>15</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="E17" s="11">
-        <v>2</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="16" t="s">
-        <v>133</v>
+      <c r="G17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="27">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="D18" s="24"/>
+      <c r="D18" s="23" t="s">
+        <v>160</v>
+      </c>
       <c r="E18" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
       <c r="L18" s="16" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="27">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="23" t="s">
@@ -1717,56 +1770,54 @@
         <v>1</v>
       </c>
       <c r="F19" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="27">
+        <v>18</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="11">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G20" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11" t="s">
+      <c r="H20" s="11"/>
+      <c r="I20" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="J20" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="K20" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="L20" s="16" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="28.8">
-      <c r="A20" s="27">
-        <v>19</v>
-      </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="16" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="28.8">
       <c r="A21" s="27">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -1775,82 +1826,84 @@
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="21" t="s">
         <v>150</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K21" s="11"/>
       <c r="L21" s="16" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" ht="28.8">
       <c r="A22" s="27">
-        <v>21</v>
-      </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="6">
-        <v>1</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L22" s="17" t="s">
-        <v>139</v>
+        <v>20</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" s="11"/>
+      <c r="I22" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="K22" s="11"/>
+      <c r="L22" s="16" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="27">
-        <v>22</v>
-      </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="6">
         <v>1</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="7"/>
+        <v>84</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
+      <c r="K23" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="L23" s="17" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="27">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
@@ -1859,24 +1912,24 @@
         <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>70</v>
+        <v>96</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>141</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>124</v>
+        <v>11</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="27">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
@@ -1885,12 +1938,14 @@
         <v>1</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="H25" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
@@ -1898,15 +1953,43 @@
         <v>140</v>
       </c>
     </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="27">
+        <v>24</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="6">
+        <v>1</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L1" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}"/>
+  <mergeCells count="1">
+    <mergeCell ref="I11:J11"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="I10" r:id="rId1" xr:uid="{134792E2-B64E-4FBB-BFC7-EC447106886D}"/>
-    <hyperlink ref="I20" r:id="rId2" xr:uid="{23725F89-30D6-47FA-ACEA-6838D1632F0F}"/>
-    <hyperlink ref="I21" r:id="rId3" xr:uid="{08EB66B2-5D49-472B-B4A7-8BD244E39350}"/>
+    <hyperlink ref="I21" r:id="rId2" xr:uid="{23725F89-30D6-47FA-ACEA-6838D1632F0F}"/>
+    <hyperlink ref="I22" r:id="rId3" xr:uid="{08EB66B2-5D49-472B-B4A7-8BD244E39350}"/>
+    <hyperlink ref="I11" r:id="rId4" display="Multiple, such as: https://www.amazon.com/Heatsink-14x14x10mm-0-55x0-55x0-39-Conductive-Dissipation/dp/B07ZC68LNM/" xr:uid="{5FD644F6-19A2-4D0C-BDC2-C003DADB325A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
BOM cost info added
</commit_message>
<xml_diff>
--- a/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
+++ b/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2 archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107BEB2F-C1C1-41AD-A42D-4D2F93DE04FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1D154A-DDE6-43EA-A6E1-3CE39152C671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
+    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'0.2 Export'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$M$26</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="203">
   <si>
     <t>Value</t>
   </si>
@@ -118,12 +118,6 @@
     <t>74LVC07</t>
   </si>
   <si>
-    <t>0805</t>
-  </si>
-  <si>
-    <t>RES-0805-1K</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -151,12 +145,6 @@
     <t>Manuf</t>
   </si>
   <si>
-    <t>MPN</t>
-  </si>
-  <si>
-    <t>DigiKey PN</t>
-  </si>
-  <si>
     <t>CKN9092-ND</t>
   </si>
   <si>
@@ -172,39 +160,24 @@
     <t>SSL-LX3044GD</t>
   </si>
   <si>
-    <t>Teensy 4.1 w/ Ethernet</t>
-  </si>
-  <si>
     <t>J1B1211CCD</t>
   </si>
   <si>
-    <t>100 µF Tantalum Cap 10 V 1206</t>
-  </si>
-  <si>
     <t>CONN JACK 1PORT 100 BASE-T PCB</t>
   </si>
   <si>
-    <t>SO20W/N</t>
-  </si>
-  <si>
     <t>RJ-45 w/ Transformer</t>
   </si>
   <si>
     <t>1849-1000-ND</t>
   </si>
   <si>
-    <t>CONN HEADER VERT 6POS 2MM</t>
-  </si>
-  <si>
     <t>1278-1052-ND</t>
   </si>
   <si>
     <t>Cetus/WIZNet</t>
   </si>
   <si>
-    <t>CAP CER 0.1UF 50V X7R</t>
-  </si>
-  <si>
     <t>SWITCH-MOMENTARY-2PTH</t>
   </si>
   <si>
@@ -394,9 +367,6 @@
     <t>A/3216-18W  1206</t>
   </si>
   <si>
-    <t>OSH Park</t>
-  </si>
-  <si>
     <t>TeensyROM v0.2</t>
   </si>
   <si>
@@ -410,12 +380,6 @@
   </si>
   <si>
     <t>2 layer 0.063" PCB</t>
-  </si>
-  <si>
-    <t>1206</t>
-  </si>
-  <si>
-    <t>Gold Fingers</t>
   </si>
   <si>
     <t>Nexperia
@@ -433,10 +397,6 @@
 296-13632-1-ND</t>
   </si>
   <si>
-    <t>Octal BUS TRANSCEIVER, 3-state
-Recommend wide package, but any of these 3 will work</t>
-  </si>
-  <si>
     <t>CONN RCPT 6POS 0.079 PCB</t>
   </si>
   <si>
@@ -455,18 +415,6 @@
     <t>For Teensy main connections to TeensyROM</t>
   </si>
   <si>
-    <t>CONN HEADER VERT 1x5 POS 0.1"</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 1x24 POS 0.1"</t>
-  </si>
-  <si>
-    <t>22-100uF CPOL-USE2.5-6</t>
-  </si>
-  <si>
-    <t>Used 22uF in protos</t>
-  </si>
-  <si>
     <t>Not required</t>
   </si>
   <si>
@@ -489,9 +437,6 @@
   </si>
   <si>
     <t>U1-Rcpt 4</t>
-  </si>
-  <si>
-    <t>Sq hole/short lead/flat side/-/Cathode</t>
   </si>
   <si>
     <t>Teensy 4.1 Devel Board w/ Ethernet</t>
@@ -593,17 +538,190 @@
     <t>14x14mm Aluminum heatsink w/ Thermal Conductive Adhesive Tape</t>
   </si>
   <si>
-    <t>Multiple, such as:     https://www.amazon.com/Heatsink-14x14x10mm-0-55x0-55x0-39-Conductive-Dissipation/dp/B07ZC68LNM/</t>
-  </si>
-  <si>
     <t>Optional, but recommended</t>
+  </si>
+  <si>
+    <t>Extended Cost (USD)</t>
+  </si>
+  <si>
+    <t>1568-DEV-16771-ND</t>
+  </si>
+  <si>
+    <t>CRG0805F1K0</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>A106056CT-ND</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>CAP 0805 CER 0.1UF 50V X7R</t>
+  </si>
+  <si>
+    <t>RES 0805 1K</t>
+  </si>
+  <si>
+    <t>74LCV245, SO20W/N</t>
+  </si>
+  <si>
+    <t>74LVC07, SO14</t>
+  </si>
+  <si>
+    <t>SW-MOM-TACTILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tantalum Cap 10 V 1206  100 µF </t>
+  </si>
+  <si>
+    <t>C64-EXPANSION-PORT Gold Fingers</t>
+  </si>
+  <si>
+    <t>CL21B104KBCNNNC</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>1276-1003-1-ND</t>
+  </si>
+  <si>
+    <t>DigiKey PN/link</t>
+  </si>
+  <si>
+    <t>P19523CT-ND</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>PJRC</t>
+  </si>
+  <si>
+    <t>ECA-1EM220I</t>
+  </si>
+  <si>
+    <t>22-100uF CPOL-US E2.5-6
+Radial Electrolytic Cap</t>
+  </si>
+  <si>
+    <t>Observe polarity</t>
+  </si>
+  <si>
+    <t>Polarity: Sq hole/short lead/flat side/-/Cathode</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 6POS (2x3) 2MM</t>
+  </si>
+  <si>
+    <t>PR20C03VBDN</t>
+  </si>
+  <si>
+    <t>Würth</t>
+  </si>
+  <si>
+    <t>61302411121</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 1x24 POS 2.54mm (0.1")</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 1x5 POS 2.54mm (0.1")</t>
+  </si>
+  <si>
+    <t>732-5331-ND</t>
+  </si>
+  <si>
+    <t>61300511121</t>
+  </si>
+  <si>
+    <t>732-5318-ND</t>
+  </si>
+  <si>
+    <t>Cost ea (USD) July 2023</t>
+  </si>
+  <si>
+    <t>10% S&amp;H</t>
+  </si>
+  <si>
+    <t>Parts total</t>
+  </si>
+  <si>
+    <t>Raw Total:</t>
+  </si>
+  <si>
+    <t>Total: Assembled and tested</t>
+  </si>
+  <si>
+    <t>Plus shipping</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hand Assy+test</t>
+  </si>
+  <si>
+    <r>
+      <t>MPN</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Highlighted=No Sub</t>
+    </r>
+  </si>
+  <si>
+    <t>Hex BUFFER, open collector HV output</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Octal Bus Transceiver, 3-state
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Recommend wide package, but any of these 3 will work</t>
+    </r>
+  </si>
+  <si>
+    <t>OSH Park prefered</t>
+  </si>
+  <si>
+    <t>2223-HSB03-141406-ND</t>
+  </si>
+  <si>
+    <t>Multiple subs, such as these w/ thermal tape attached</t>
+  </si>
+  <si>
+    <t>CUI Devices HSB03-141406 (+ therm tape)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -638,8 +756,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -682,8 +815,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -719,25 +864,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -819,11 +952,75 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1137,11 +1334,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L26"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1151,26 +1348,27 @@
     <col min="5" max="5" width="3.77734375" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.109375" style="9" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="24.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.44140625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="21" style="9" customWidth="1"/>
-    <col min="12" max="12" width="35.77734375" style="9" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="9"/>
+    <col min="8" max="8" width="24.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" style="32" customWidth="1"/>
+    <col min="13" max="13" width="35.77734375" style="9" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="15" customFormat="1" ht="28.8">
+    <row r="1" spans="1:13" s="15" customFormat="1" ht="28.8">
       <c r="A1" s="26" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>18</v>
@@ -1182,67 +1380,79 @@
         <v>0</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>35</v>
+        <v>196</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>171</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="27">
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>108</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>160</v>
+      </c>
+      <c r="K2" s="34">
+        <f>32.4/3</f>
+        <v>10.799999999999999</v>
+      </c>
+      <c r="L2" s="34">
+        <f t="shared" ref="L2:L17" si="0">K2*E2</f>
+        <v>10.799999999999999</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="27">
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E3" s="5">
         <v>2</v>
@@ -1251,58 +1461,78 @@
         <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="1:12">
+        <v>162</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="K3" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="34">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="27">
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E4" s="5">
         <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="H4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" ht="43.2">
+        <v>169</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="K4" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="34">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="1:13" ht="43.2">
       <c r="A5" s="27">
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E5" s="5">
         <v>4</v>
@@ -1311,36 +1541,40 @@
         <v>23</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="28.8">
+        <v>113</v>
+      </c>
+      <c r="I5" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="K5" s="34">
+        <v>0.68</v>
+      </c>
+      <c r="L5" s="34">
+        <f t="shared" si="0"/>
+        <v>2.72</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="27">
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -1349,72 +1583,80 @@
         <v>17</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="I6" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="34">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="27">
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>2</v>
+        <v>165</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="1:12">
+        <v>36</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="34">
+        <v>0.19</v>
+      </c>
+      <c r="L7" s="34">
+        <f t="shared" si="0"/>
+        <v>0.19</v>
+      </c>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" ht="28.8">
       <c r="A8" s="27">
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
@@ -1426,33 +1668,37 @@
         <v>6</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>38</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="34">
+        <v>0.43</v>
+      </c>
+      <c r="L8" s="34">
+        <f t="shared" si="0"/>
+        <v>0.43</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="28.8">
       <c r="A9" s="27">
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E9" s="5">
         <v>2</v>
@@ -1461,30 +1707,40 @@
         <v>20</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="28.8">
+        <v>173</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="K9" s="34">
+        <v>0.22</v>
+      </c>
+      <c r="L9" s="34">
+        <f t="shared" si="0"/>
+        <v>0.44</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="28.8">
       <c r="A10" s="27">
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -1493,217 +1749,283 @@
         <v>15</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="H10" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="I10" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="28.8">
+      <c r="J10" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="K10" s="34">
+        <v>33.08</v>
+      </c>
+      <c r="L10" s="34">
+        <f t="shared" si="0"/>
+        <v>33.08</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="28.8" customHeight="1">
       <c r="A11" s="27" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E11" s="5">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="28.8">
+        <v>153</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="K11" s="34">
+        <v>0.74</v>
+      </c>
+      <c r="L11" s="34">
+        <f t="shared" si="0"/>
+        <v>0.74</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="28.8">
       <c r="A12" s="27">
         <v>10</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E12" s="8">
         <v>2</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="43.2">
+        <v>183</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="K12" s="34">
+        <v>1.31</v>
+      </c>
+      <c r="L12" s="34">
+        <f t="shared" si="0"/>
+        <v>2.62</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="43.2">
       <c r="A13" s="27">
         <v>11</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E13" s="8">
         <v>1</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="24" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="43.2">
+        <v>184</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="K13" s="34">
+        <v>0.26</v>
+      </c>
+      <c r="L13" s="34">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="M13" s="24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="43.2">
       <c r="A14" s="27">
         <v>12</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E14" s="8">
         <v>1</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="L14" s="24" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>179</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="34">
+        <v>0.19</v>
+      </c>
+      <c r="L14" s="34">
+        <f t="shared" si="0"/>
+        <v>0.19</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="27">
         <v>13</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="5">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>53</v>
+        <v>161</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-    </row>
-    <row r="16" spans="1:12">
+        <v>169</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="K15" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="L15" s="34">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="27">
         <v>14</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="5">
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="I16" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="34">
+        <v>3.78</v>
+      </c>
+      <c r="L16" s="34">
+        <f t="shared" si="0"/>
+        <v>3.78</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="27">
         <v>15</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="5">
@@ -1713,165 +2035,176 @@
         <v>16</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>28</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I17" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="J17" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" s="34">
+        <v>1.61</v>
+      </c>
+      <c r="L17" s="34">
+        <f t="shared" si="0"/>
+        <v>1.61</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" hidden="1">
       <c r="A18" s="27">
         <v>16</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E18" s="11">
         <v>2</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" hidden="1">
       <c r="A19" s="27">
         <v>17</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="11">
         <v>1</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" hidden="1">
       <c r="A20" s="27">
         <v>18</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="11">
         <v>1</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="H20" s="11"/>
+        <v>116</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>117</v>
+      </c>
       <c r="I20" s="11" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="28.8">
+        <v>119</v>
+      </c>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="28.8" hidden="1">
       <c r="A21" s="27">
         <v>19</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
       <c r="D21" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="28.8">
+        <v>133</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="J21" s="11"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="28.8" hidden="1">
       <c r="A22" s="27">
         <v>20</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
       <c r="D22" s="23" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="K22" s="11"/>
-      <c r="L22" s="16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>134</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" hidden="1">
       <c r="A23" s="27">
         <v>21</v>
       </c>
@@ -1882,26 +2215,25 @@
         <v>1</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L23" s="17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>166</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" hidden="1">
       <c r="A24" s="27">
         <v>22</v>
       </c>
@@ -1912,22 +2244,21 @@
         <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>11</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" hidden="1">
       <c r="A25" s="27">
         <v>23</v>
       </c>
@@ -1938,22 +2269,21 @@
         <v>1</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>124</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" hidden="1">
       <c r="A26" s="27">
         <v>24</v>
       </c>
@@ -1964,32 +2294,117 @@
         <v>1</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="17" t="s">
-        <v>140</v>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="45" customFormat="1" ht="6.6" customHeight="1">
+      <c r="A27" s="44"/>
+      <c r="E27" s="46"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="47"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="K28" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="L28" s="42">
+        <f>SUM(L2:L26)</f>
+        <v>58.16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="K29" s="48" t="s">
+        <v>189</v>
+      </c>
+      <c r="L29" s="32">
+        <f>L28*10%</f>
+        <v>5.8159999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="K30" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="L30" s="37">
+        <f>L29+L28</f>
+        <v>63.975999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="K31" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="L31" s="32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="J32" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="K32" s="50"/>
+      <c r="L32" s="37">
+        <f>L31+L30</f>
+        <v>78.975999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="10:12">
+      <c r="J33" s="43"/>
+      <c r="K33" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="L33" s="36" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}"/>
+  <autoFilter ref="A1:M26" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="J32:K32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I10" r:id="rId1" xr:uid="{134792E2-B64E-4FBB-BFC7-EC447106886D}"/>
-    <hyperlink ref="I21" r:id="rId2" xr:uid="{23725F89-30D6-47FA-ACEA-6838D1632F0F}"/>
-    <hyperlink ref="I22" r:id="rId3" xr:uid="{08EB66B2-5D49-472B-B4A7-8BD244E39350}"/>
-    <hyperlink ref="I11" r:id="rId4" display="Multiple, such as: https://www.amazon.com/Heatsink-14x14x10mm-0-55x0-55x0-39-Conductive-Dissipation/dp/B07ZC68LNM/" xr:uid="{5FD644F6-19A2-4D0C-BDC2-C003DADB325A}"/>
+    <hyperlink ref="H10" r:id="rId1" display="https://www.pjrc.com/store" xr:uid="{134792E2-B64E-4FBB-BFC7-EC447106886D}"/>
+    <hyperlink ref="H21" r:id="rId2" xr:uid="{23725F89-30D6-47FA-ACEA-6838D1632F0F}"/>
+    <hyperlink ref="H22" r:id="rId3" xr:uid="{08EB66B2-5D49-472B-B4A7-8BD244E39350}"/>
+    <hyperlink ref="H11" r:id="rId4" display="Multiple, such as: https://www.amazon.com/Heatsink-14x14x10mm-0-55x0-55x0-39-Conductive-Dissipation/dp/B07ZC68LNM/" xr:uid="{5FD644F6-19A2-4D0C-BDC2-C003DADB325A}"/>
+    <hyperlink ref="J5" r:id="rId5" display="https://www.digikey.com/en/products/detail/nexperia-usa-inc/74LVC245AD-118/946690" xr:uid="{58DCABB5-EDC7-4E2D-A244-D34D14A1826B}"/>
+    <hyperlink ref="I10" r:id="rId6" xr:uid="{8F740FC1-EDF0-4C9E-9823-C987C0E04A4F}"/>
+    <hyperlink ref="J10" r:id="rId7" xr:uid="{0DE6FCC4-E35A-47FB-9DC7-F030B4E296C0}"/>
+    <hyperlink ref="J6" r:id="rId8" xr:uid="{E5BB0DA3-B914-4FF4-B66E-5980E82AA257}"/>
+    <hyperlink ref="I2" r:id="rId9" xr:uid="{73C4327B-52E7-45DC-881A-E0847ED73C61}"/>
+    <hyperlink ref="J3" r:id="rId10" xr:uid="{D713217F-486F-4E73-A804-2166CA542C2D}"/>
+    <hyperlink ref="J4" r:id="rId11" xr:uid="{00640734-08BA-4F39-8C8E-D0CF6E96C735}"/>
+    <hyperlink ref="J7" r:id="rId12" xr:uid="{6F229ED7-CAEA-4D67-BFF0-0E0AA066F8B2}"/>
+    <hyperlink ref="J8" r:id="rId13" xr:uid="{FE4A259F-8D56-43F3-928F-E2509BF332B9}"/>
+    <hyperlink ref="J9" r:id="rId14" xr:uid="{5AA0053B-4694-45A0-990D-299A2E63F143}"/>
+    <hyperlink ref="J15" r:id="rId15" xr:uid="{0EF3ADE5-4B57-406C-BDCD-A5AD446D9733}"/>
+    <hyperlink ref="J16" r:id="rId16" xr:uid="{B7489C6B-4B67-493F-A4BC-72AA11902DA0}"/>
+    <hyperlink ref="J17" r:id="rId17" xr:uid="{0F65CBF2-C3AE-4742-BDAA-ADF047E394C6}"/>
+    <hyperlink ref="J14" r:id="rId18" xr:uid="{4E963CB5-4BC8-4A66-A683-2D131B96C08C}"/>
+    <hyperlink ref="J12" r:id="rId19" xr:uid="{890A73F3-E6DD-4DD6-A06E-81924A5413A3}"/>
+    <hyperlink ref="J13" r:id="rId20" xr:uid="{DF130F23-5B34-41D1-86C6-D27E2C2FCFE8}"/>
+    <hyperlink ref="J11" r:id="rId21" xr:uid="{E52F636D-3699-4616-A972-2410D7682974}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -2032,40 +2447,40 @@
         <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -2073,19 +2488,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -2102,10 +2517,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -2114,28 +2529,28 @@
         <v>805</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -2143,19 +2558,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -2172,7 +2587,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -2184,24 +2599,24 @@
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -2209,16 +2624,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2240,13 +2655,13 @@
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -2263,29 +2678,29 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -2296,19 +2711,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -2325,16 +2740,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2352,19 +2767,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -2384,10 +2799,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>3</v>
@@ -2441,10 +2856,10 @@
         <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>8</v>
@@ -2470,7 +2885,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
R3 added to BOM
</commit_message>
<xml_diff>
--- a/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
+++ b/PCB/v0.2 archive/TeensyROM v0.2 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2 archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1D154A-DDE6-43EA-A6E1-3CE39152C671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D99F1B-6454-4F13-9E8C-D75AFFEA2D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'0.2 Export'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$M$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$M$27</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="209">
   <si>
     <t>Value</t>
   </si>
@@ -712,6 +712,24 @@
   </si>
   <si>
     <t>CUI Devices HSB03-141406 (+ therm tape)</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>RES 0805 10K</t>
+  </si>
+  <si>
+    <t>CRG0805F10K</t>
+  </si>
+  <si>
+    <t>A106054CT-ND</t>
+  </si>
+  <si>
+    <t>Locations/RefDes</t>
   </si>
 </sst>
 </file>
@@ -1334,11 +1352,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:M33"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1374,7 +1392,7 @@
         <v>18</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>19</v>
+        <v>208</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>0</v>
@@ -1434,7 +1452,7 @@
         <v>10.799999999999999</v>
       </c>
       <c r="L2" s="34">
-        <f t="shared" ref="L2:L17" si="0">K2*E2</f>
+        <f t="shared" ref="L2:L18" si="0">K2*E2</f>
         <v>10.799999999999999</v>
       </c>
       <c r="M2" s="8" t="s">
@@ -1482,544 +1500,544 @@
       <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="27">
+      <c r="A4" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="K4" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="34">
+        <f t="shared" ref="L4" si="1">K4*E4</f>
+        <v>0.1</v>
+      </c>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="27">
         <v>3</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="B5" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="5">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J5" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="K4" s="35">
+      <c r="K5" s="35">
         <v>0.1</v>
       </c>
-      <c r="L4" s="34">
+      <c r="L5" s="34">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="M4" s="10"/>
-    </row>
-    <row r="5" spans="1:13" ht="43.2">
-      <c r="A5" s="27">
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="1:13" ht="43.2">
+      <c r="A6" s="27">
         <v>4</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" s="5">
+      <c r="B6" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="5">
         <v>4</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="I5" s="41" t="s">
+      <c r="I6" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J6" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K6" s="34">
         <v>0.68</v>
       </c>
-      <c r="L5" s="34">
+      <c r="L6" s="34">
         <f t="shared" si="0"/>
         <v>2.72</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M6" s="8" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="27">
+    <row r="7" spans="1:13">
+      <c r="A7" s="27">
         <v>5</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="B7" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" s="5">
         <v>1</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="41" t="s">
+      <c r="I7" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J7" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K7" s="34">
         <v>0.5</v>
       </c>
-      <c r="L6" s="34">
+      <c r="L7" s="34">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="27">
+    <row r="8" spans="1:13">
+      <c r="A8" s="27">
         <v>6</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="B8" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J8" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K8" s="34">
         <v>0.19</v>
       </c>
-      <c r="L7" s="34">
+      <c r="L8" s="34">
         <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:13" ht="28.8">
-      <c r="A8" s="27">
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" ht="28.8">
+      <c r="A9" s="27">
         <v>7</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="B9" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="J9" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="K8" s="34">
+      <c r="K9" s="34">
         <v>0.43</v>
       </c>
-      <c r="L8" s="34">
+      <c r="L9" s="34">
         <f t="shared" si="0"/>
         <v>0.43</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="M9" s="8" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="28.8">
-      <c r="A9" s="27">
+    <row r="10" spans="1:13" ht="28.8">
+      <c r="A10" s="27">
         <v>8</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E9" s="5">
+      <c r="B10" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" s="5">
         <v>2</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H10" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I10" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J10" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K10" s="34">
         <v>0.22</v>
       </c>
-      <c r="L9" s="34">
+      <c r="L10" s="34">
         <f t="shared" si="0"/>
         <v>0.44</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="M10" s="8" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="28.8">
-      <c r="A10" s="27">
+    <row r="11" spans="1:13" ht="28.8">
+      <c r="A11" s="27">
         <v>9</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="B11" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H11" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="I10" s="40" t="s">
+      <c r="I11" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J11" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K11" s="34">
         <v>33.08</v>
       </c>
-      <c r="L10" s="34">
+      <c r="L11" s="34">
         <f t="shared" si="0"/>
         <v>33.08</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M11" s="19" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="28.8" customHeight="1">
-      <c r="A11" s="27" t="s">
+    <row r="12" spans="1:13" ht="28.8" customHeight="1">
+      <c r="A12" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="5">
+      <c r="B12" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H12" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I12" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J12" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K12" s="34">
         <v>0.74</v>
       </c>
-      <c r="L11" s="34">
+      <c r="L12" s="34">
         <f t="shared" si="0"/>
         <v>0.74</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="28.8">
-      <c r="A12" s="27">
+    <row r="13" spans="1:13" ht="28.8">
+      <c r="A13" s="27">
         <v>10</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E12" s="8">
+      <c r="B13" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" s="8">
         <v>2</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I13" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="J13" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="K12" s="34">
+      <c r="K13" s="34">
         <v>1.31</v>
       </c>
-      <c r="L12" s="34">
+      <c r="L13" s="34">
         <f t="shared" si="0"/>
         <v>2.62</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="M13" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.2">
-      <c r="A13" s="27">
+    <row r="14" spans="1:13" ht="43.2">
+      <c r="A14" s="27">
         <v>11</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" s="8">
+      <c r="B14" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" s="8">
         <v>1</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I14" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J14" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="K13" s="34">
+      <c r="K14" s="34">
         <v>0.26</v>
       </c>
-      <c r="L13" s="34">
+      <c r="L14" s="34">
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="M13" s="24" t="s">
+      <c r="M14" s="24" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="43.2">
-      <c r="A14" s="27">
+    <row r="15" spans="1:13" ht="43.2">
+      <c r="A15" s="27">
         <v>12</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E14" s="8">
+      <c r="B15" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="8">
         <v>1</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F15" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G15" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H15" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I15" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J15" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="K14" s="34">
+      <c r="K15" s="34">
         <v>0.19</v>
       </c>
-      <c r="L14" s="34">
+      <c r="L15" s="34">
         <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
-      <c r="M14" s="24" t="s">
+      <c r="M15" s="24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="27">
+    <row r="16" spans="1:13">
+      <c r="A16" s="27">
         <v>13</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="5">
+      <c r="B16" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="5">
         <v>1</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H16" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I16" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="J15" s="38" t="s">
+      <c r="J16" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="K15" s="35">
+      <c r="K16" s="35">
         <v>0.1</v>
       </c>
-      <c r="L15" s="34">
+      <c r="L16" s="34">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="M15" s="10"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="27">
-        <v>14</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="5">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="K16" s="34">
-        <v>3.78</v>
-      </c>
-      <c r="L16" s="34">
-        <f t="shared" si="0"/>
-        <v>3.78</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>40</v>
-      </c>
+      <c r="M16" s="10"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="27">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>142</v>
@@ -2032,77 +2050,90 @@
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="I17" s="41" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="J17" s="39" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="K17" s="34">
-        <v>1.61</v>
+        <v>3.78</v>
       </c>
       <c r="L17" s="34">
         <f t="shared" si="0"/>
+        <v>3.78</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="27">
+        <v>15</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="34">
         <v>1.61</v>
       </c>
-      <c r="M17" s="8" t="s">
+      <c r="L18" s="34">
+        <f t="shared" si="0"/>
+        <v>1.61</v>
+      </c>
+      <c r="M18" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1">
-      <c r="A18" s="27">
+    <row r="19" spans="1:13">
+      <c r="A19" s="27">
         <v>16</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E18" s="11">
-        <v>2</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" hidden="1">
-      <c r="A19" s="27">
-        <v>17</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="D19" s="24"/>
+      <c r="D19" s="23" t="s">
+        <v>142</v>
+      </c>
       <c r="E19" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
@@ -2110,12 +2141,12 @@
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
       <c r="M19" s="16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" hidden="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="27">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="23" t="s">
@@ -2126,58 +2157,56 @@
         <v>1</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>119</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
       <c r="M20" s="16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="28.8" hidden="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="27">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E21" s="11"/>
+      <c r="C21" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="11">
+        <v>1</v>
+      </c>
       <c r="F21" s="11" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>132</v>
+        <v>116</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="J21" s="11"/>
+        <v>118</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>119</v>
+      </c>
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
       <c r="M21" s="16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="28.8" hidden="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="28.8">
       <c r="A22" s="27">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
@@ -2186,16 +2215,16 @@
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H22" s="21" t="s">
         <v>132</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J22" s="11"/>
       <c r="K22" s="30"/>
@@ -2204,63 +2233,67 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1">
+    <row r="23" spans="1:13" ht="28.8">
       <c r="A23" s="27">
+        <v>20</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="27">
         <v>21</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="6">
-        <v>1</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" hidden="1">
-      <c r="A24" s="27">
-        <v>22</v>
-      </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="6">
         <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="H24" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
+      <c r="J24" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
       <c r="M24" s="17" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1">
+    <row r="25" spans="1:13">
       <c r="A25" s="27">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
@@ -2269,10 +2302,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>167</v>
+        <v>87</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>124</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -2280,12 +2313,12 @@
       <c r="K25" s="31"/>
       <c r="L25" s="31"/>
       <c r="M25" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" hidden="1">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="27">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="24"/>
       <c r="C26" s="24"/>
@@ -2294,10 +2327,10 @@
         <v>1</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>48</v>
+        <v>167</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -2308,103 +2341,123 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="45" customFormat="1" ht="6.6" customHeight="1">
-      <c r="A27" s="44"/>
-      <c r="E27" s="46"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="47"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="K28" s="33" t="s">
+    <row r="27" spans="1:13">
+      <c r="A27" s="27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="45" customFormat="1" ht="6.6" customHeight="1">
+      <c r="A28" s="44"/>
+      <c r="E28" s="46"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="47"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="K29" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="L28" s="42">
-        <f>SUM(L2:L26)</f>
-        <v>58.16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="K29" s="48" t="s">
+      <c r="L29" s="42">
+        <f>SUM(L2:L27)</f>
+        <v>58.259999999999991</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="K30" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="L29" s="32">
-        <f>L28*10%</f>
-        <v>5.8159999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="K30" s="36" t="s">
+      <c r="L30" s="32">
+        <f>L29*10%</f>
+        <v>5.8259999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="K31" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="L30" s="37">
-        <f>L29+L28</f>
-        <v>63.975999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="K31" s="48" t="s">
+      <c r="L31" s="37">
+        <f>L30+L29</f>
+        <v>64.085999999999984</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="K32" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="L31" s="32">
+      <c r="L32" s="32">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
-      <c r="J32" s="50" t="s">
+    <row r="33" spans="10:12">
+      <c r="J33" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="K32" s="50"/>
-      <c r="L32" s="37">
-        <f>L31+L30</f>
-        <v>78.975999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="10:12">
-      <c r="J33" s="43"/>
-      <c r="K33" s="36" t="s">
+      <c r="K33" s="50"/>
+      <c r="L33" s="37">
+        <f>L32+L31</f>
+        <v>79.085999999999984</v>
+      </c>
+    </row>
+    <row r="34" spans="10:12">
+      <c r="J34" s="43"/>
+      <c r="K34" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="L33" s="36" t="s">
+      <c r="L34" s="36" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M26" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M27" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}"/>
   <mergeCells count="1">
-    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J33:K33"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H10" r:id="rId1" display="https://www.pjrc.com/store" xr:uid="{134792E2-B64E-4FBB-BFC7-EC447106886D}"/>
-    <hyperlink ref="H21" r:id="rId2" xr:uid="{23725F89-30D6-47FA-ACEA-6838D1632F0F}"/>
-    <hyperlink ref="H22" r:id="rId3" xr:uid="{08EB66B2-5D49-472B-B4A7-8BD244E39350}"/>
-    <hyperlink ref="H11" r:id="rId4" display="Multiple, such as: https://www.amazon.com/Heatsink-14x14x10mm-0-55x0-55x0-39-Conductive-Dissipation/dp/B07ZC68LNM/" xr:uid="{5FD644F6-19A2-4D0C-BDC2-C003DADB325A}"/>
-    <hyperlink ref="J5" r:id="rId5" display="https://www.digikey.com/en/products/detail/nexperia-usa-inc/74LVC245AD-118/946690" xr:uid="{58DCABB5-EDC7-4E2D-A244-D34D14A1826B}"/>
-    <hyperlink ref="I10" r:id="rId6" xr:uid="{8F740FC1-EDF0-4C9E-9823-C987C0E04A4F}"/>
-    <hyperlink ref="J10" r:id="rId7" xr:uid="{0DE6FCC4-E35A-47FB-9DC7-F030B4E296C0}"/>
-    <hyperlink ref="J6" r:id="rId8" xr:uid="{E5BB0DA3-B914-4FF4-B66E-5980E82AA257}"/>
+    <hyperlink ref="H11" r:id="rId1" display="https://www.pjrc.com/store" xr:uid="{134792E2-B64E-4FBB-BFC7-EC447106886D}"/>
+    <hyperlink ref="H22" r:id="rId2" xr:uid="{23725F89-30D6-47FA-ACEA-6838D1632F0F}"/>
+    <hyperlink ref="H23" r:id="rId3" xr:uid="{08EB66B2-5D49-472B-B4A7-8BD244E39350}"/>
+    <hyperlink ref="H12" r:id="rId4" display="Multiple, such as: https://www.amazon.com/Heatsink-14x14x10mm-0-55x0-55x0-39-Conductive-Dissipation/dp/B07ZC68LNM/" xr:uid="{5FD644F6-19A2-4D0C-BDC2-C003DADB325A}"/>
+    <hyperlink ref="J6" r:id="rId5" display="https://www.digikey.com/en/products/detail/nexperia-usa-inc/74LVC245AD-118/946690" xr:uid="{58DCABB5-EDC7-4E2D-A244-D34D14A1826B}"/>
+    <hyperlink ref="I11" r:id="rId6" xr:uid="{8F740FC1-EDF0-4C9E-9823-C987C0E04A4F}"/>
+    <hyperlink ref="J11" r:id="rId7" xr:uid="{0DE6FCC4-E35A-47FB-9DC7-F030B4E296C0}"/>
+    <hyperlink ref="J7" r:id="rId8" xr:uid="{E5BB0DA3-B914-4FF4-B66E-5980E82AA257}"/>
     <hyperlink ref="I2" r:id="rId9" xr:uid="{73C4327B-52E7-45DC-881A-E0847ED73C61}"/>
     <hyperlink ref="J3" r:id="rId10" xr:uid="{D713217F-486F-4E73-A804-2166CA542C2D}"/>
-    <hyperlink ref="J4" r:id="rId11" xr:uid="{00640734-08BA-4F39-8C8E-D0CF6E96C735}"/>
-    <hyperlink ref="J7" r:id="rId12" xr:uid="{6F229ED7-CAEA-4D67-BFF0-0E0AA066F8B2}"/>
-    <hyperlink ref="J8" r:id="rId13" xr:uid="{FE4A259F-8D56-43F3-928F-E2509BF332B9}"/>
-    <hyperlink ref="J9" r:id="rId14" xr:uid="{5AA0053B-4694-45A0-990D-299A2E63F143}"/>
-    <hyperlink ref="J15" r:id="rId15" xr:uid="{0EF3ADE5-4B57-406C-BDCD-A5AD446D9733}"/>
-    <hyperlink ref="J16" r:id="rId16" xr:uid="{B7489C6B-4B67-493F-A4BC-72AA11902DA0}"/>
-    <hyperlink ref="J17" r:id="rId17" xr:uid="{0F65CBF2-C3AE-4742-BDAA-ADF047E394C6}"/>
-    <hyperlink ref="J14" r:id="rId18" xr:uid="{4E963CB5-4BC8-4A66-A683-2D131B96C08C}"/>
-    <hyperlink ref="J12" r:id="rId19" xr:uid="{890A73F3-E6DD-4DD6-A06E-81924A5413A3}"/>
-    <hyperlink ref="J13" r:id="rId20" xr:uid="{DF130F23-5B34-41D1-86C6-D27E2C2FCFE8}"/>
-    <hyperlink ref="J11" r:id="rId21" xr:uid="{E52F636D-3699-4616-A972-2410D7682974}"/>
+    <hyperlink ref="J5" r:id="rId11" xr:uid="{00640734-08BA-4F39-8C8E-D0CF6E96C735}"/>
+    <hyperlink ref="J8" r:id="rId12" xr:uid="{6F229ED7-CAEA-4D67-BFF0-0E0AA066F8B2}"/>
+    <hyperlink ref="J9" r:id="rId13" xr:uid="{FE4A259F-8D56-43F3-928F-E2509BF332B9}"/>
+    <hyperlink ref="J10" r:id="rId14" xr:uid="{5AA0053B-4694-45A0-990D-299A2E63F143}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{0EF3ADE5-4B57-406C-BDCD-A5AD446D9733}"/>
+    <hyperlink ref="J17" r:id="rId16" xr:uid="{B7489C6B-4B67-493F-A4BC-72AA11902DA0}"/>
+    <hyperlink ref="J18" r:id="rId17" xr:uid="{0F65CBF2-C3AE-4742-BDAA-ADF047E394C6}"/>
+    <hyperlink ref="J15" r:id="rId18" xr:uid="{4E963CB5-4BC8-4A66-A683-2D131B96C08C}"/>
+    <hyperlink ref="J13" r:id="rId19" xr:uid="{890A73F3-E6DD-4DD6-A06E-81924A5413A3}"/>
+    <hyperlink ref="J14" r:id="rId20" xr:uid="{DF130F23-5B34-41D1-86C6-D27E2C2FCFE8}"/>
+    <hyperlink ref="J12" r:id="rId21" xr:uid="{E52F636D-3699-4616-A972-2410D7682974}"/>
+    <hyperlink ref="J4" r:id="rId22" xr:uid="{BFF33686-00DA-47D6-B57E-31FEFD3C8B56}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId22"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
 </worksheet>
 </file>
 

</xml_diff>